<commit_message>
leuven update thinking centOS7 partition
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2.xlsx
+++ b/source/leuven/tier2_hardware/thinking_hardware/thinking_node_map_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geert\Documents\Data\GitHub\VscDocumentation\source\leuven\tier2_hardware\thinking_hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\HPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5775" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="5780" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="node_map" sheetId="1" r:id="rId1"/>
@@ -481,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -541,6 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,23 +896,23 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="1" customWidth="1"/>
-    <col min="2" max="17" width="3.85546875" customWidth="1"/>
-    <col min="18" max="18" width="6.28515625" customWidth="1"/>
-    <col min="19" max="20" width="3.5703125" customWidth="1"/>
-    <col min="21" max="23" width="11.5703125"/>
-    <col min="24" max="24" width="14.7109375" customWidth="1"/>
-    <col min="25" max="26" width="11.5703125"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="8.453125" style="1" customWidth="1"/>
+    <col min="2" max="17" width="3.81640625" customWidth="1"/>
+    <col min="18" max="18" width="6.26953125" customWidth="1"/>
+    <col min="19" max="20" width="3.54296875" customWidth="1"/>
+    <col min="21" max="23" width="11.54296875"/>
+    <col min="24" max="24" width="14.7265625" customWidth="1"/>
+    <col min="25" max="26" width="11.54296875"/>
+    <col min="27" max="27" width="14.81640625" customWidth="1"/>
+    <col min="28" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -961,7 +962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -982,7 +983,7 @@
       <c r="P2" s="18"/>
       <c r="Q2" s="18"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1003,7 +1004,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -1024,7 +1025,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1033,7 +1034,7 @@
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -1045,7 +1046,7 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1087,11 +1088,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
@@ -1130,7 +1131,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1146,10 +1147,10 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
+      <c r="N8" s="43"/>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
+      <c r="Q8" s="43"/>
       <c r="S8" s="8"/>
       <c r="T8" s="9"/>
       <c r="U8" t="s">
@@ -1172,7 +1173,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1180,13 +1181,13 @@
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
@@ -1214,11 +1215,11 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1257,7 +1258,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1345,7 +1346,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1366,7 +1367,7 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1416,7 @@
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
     </row>
-    <row r="16" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1461,7 +1462,7 @@
       <c r="P17" s="32"/>
       <c r="Q17" s="33"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
@@ -1482,7 +1483,7 @@
       <c r="P18" s="21"/>
       <c r="Q18" s="35"/>
     </row>
-    <row r="19" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
@@ -1503,7 +1504,7 @@
       <c r="P19" s="21"/>
       <c r="Q19" s="35"/>
     </row>
-    <row r="20" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
@@ -1573,7 +1574,7 @@
       <c r="P22" s="21"/>
       <c r="Q22" s="35"/>
     </row>
-    <row r="23" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="P23" s="37"/>
       <c r="Q23" s="38"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1614,7 +1615,7 @@
       <c r="Q24" s="24"/>
       <c r="R24" s="25"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="13" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1648,7 +1649,7 @@
       <c r="Q25" s="28"/>
       <c r="R25" s="29"/>
     </row>
-    <row r="26" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" s="9" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
@@ -1670,7 +1671,7 @@
       <c r="Q26" s="28"/>
       <c r="R26" s="29"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>

</xml_diff>